<commit_message>
updates to manuscript and figures
</commit_message>
<xml_diff>
--- a/Randomisation/Final_Randomisation.xlsx
+++ b/Randomisation/Final_Randomisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saoirsekelleher/Documents/Research/QAEco/DOM_Review/Randomisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7C87AC-BB34-1C4E-862B-2E0859CDAFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CF4A3C-BB8D-2C4D-9E71-97AF825625E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{3B957EFC-CA0F-9A4A-8B5B-5DFB75D21C9C}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7457" uniqueCount="4581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7542" uniqueCount="4581">
   <si>
     <t>Review_ID</t>
   </si>
@@ -13804,7 +13804,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -13938,12 +13938,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -14446,11 +14440,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -14461,16 +14455,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -14501,6 +14485,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -14850,8 +14844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085D3674-2ED6-F04D-977B-AC5353E9040B}">
   <dimension ref="A1:L1470"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15583,6 +15577,9 @@
       <c r="K19" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L19" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
@@ -15618,6 +15615,9 @@
       <c r="K20" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L20" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
@@ -15653,6 +15653,9 @@
       <c r="K21" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L21" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
@@ -15688,6 +15691,9 @@
       <c r="K22" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L22" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
@@ -15723,6 +15729,9 @@
       <c r="K23" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L23" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
@@ -15758,6 +15767,9 @@
       <c r="K24" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L24" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
@@ -15793,6 +15805,9 @@
       <c r="K25" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L25" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
@@ -15828,6 +15843,9 @@
       <c r="K26" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L26" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
@@ -15863,6 +15881,9 @@
       <c r="K27" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L27" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
@@ -15898,6 +15919,9 @@
       <c r="K28" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L28" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
@@ -15933,6 +15957,9 @@
       <c r="K29" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L29" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
@@ -15968,6 +15995,9 @@
       <c r="K30" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L30" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
@@ -16003,6 +16033,9 @@
       <c r="K31" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L31" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
@@ -16038,8 +16071,11 @@
       <c r="K32" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L32" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>754</v>
       </c>
@@ -16073,8 +16109,11 @@
       <c r="K33" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L33" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>796</v>
       </c>
@@ -16108,8 +16147,11 @@
       <c r="K34" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L34" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>1260</v>
       </c>
@@ -16143,8 +16185,11 @@
       <c r="K35" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L35" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>583</v>
       </c>
@@ -16178,8 +16223,11 @@
       <c r="K36" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L36" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>47</v>
       </c>
@@ -16213,8 +16261,11 @@
       <c r="K37" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L37" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>42</v>
       </c>
@@ -16248,8 +16299,11 @@
       <c r="K38" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L38" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>575</v>
       </c>
@@ -16283,8 +16337,11 @@
       <c r="K39" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L39" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>337</v>
       </c>
@@ -16318,8 +16375,11 @@
       <c r="K40" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L40" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>870</v>
       </c>
@@ -16353,8 +16413,11 @@
       <c r="K41" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L41" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>37</v>
       </c>
@@ -16388,8 +16451,11 @@
       <c r="K42" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L42" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>1065</v>
       </c>
@@ -16423,8 +16489,11 @@
       <c r="K43" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L43" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>1150</v>
       </c>
@@ -16458,8 +16527,11 @@
       <c r="K44" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L44" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>773</v>
       </c>
@@ -16493,8 +16565,11 @@
       <c r="K45" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L45" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>3</v>
       </c>
@@ -16528,8 +16603,11 @@
       <c r="K46" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L46" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>812</v>
       </c>
@@ -16563,8 +16641,11 @@
       <c r="K47" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L47" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>642</v>
       </c>
@@ -16598,8 +16679,11 @@
       <c r="K48" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L48" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>17</v>
       </c>
@@ -16633,8 +16717,11 @@
       <c r="K49" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L49" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>725</v>
       </c>
@@ -16668,8 +16755,11 @@
       <c r="K50" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L50" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>700</v>
       </c>
@@ -16703,8 +16793,11 @@
       <c r="K51" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L51" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>617</v>
       </c>
@@ -16738,8 +16831,11 @@
       <c r="K52" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L52" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>907</v>
       </c>
@@ -16773,8 +16869,11 @@
       <c r="K53" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L53" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>240</v>
       </c>
@@ -16808,8 +16907,11 @@
       <c r="K54" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L54" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>589</v>
       </c>
@@ -16844,7 +16946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>91</v>
       </c>
@@ -16879,7 +16981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>683</v>
       </c>
@@ -16914,7 +17016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>199</v>
       </c>
@@ -16949,7 +17051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>608</v>
       </c>
@@ -16984,7 +17086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>49</v>
       </c>
@@ -17019,7 +17121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>663</v>
       </c>
@@ -17054,7 +17156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>572</v>
       </c>
@@ -17089,7 +17191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>1382</v>
       </c>
@@ -17124,7 +17226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>336</v>
       </c>
@@ -19477,14 +19579,14 @@
     <row r="1470" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
-      <formula>"YES"</formula>
+    <cfRule type="containsBlanks" dxfId="14" priority="1">
+      <formula>LEN(TRIM(L2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="12" priority="1">
-      <formula>LEN(TRIM(L2))=0</formula>
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+      <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -19500,8 +19602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719613DA-2E8B-AC4E-A768-CCAA40374210}">
   <dimension ref="A1:L213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20344,6 +20446,9 @@
       <c r="K22" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L22" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
@@ -20379,6 +20484,9 @@
       <c r="K23" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L23" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
@@ -20414,6 +20522,9 @@
       <c r="K24" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L24" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
@@ -20449,6 +20560,9 @@
       <c r="K25" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L25" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
@@ -20484,6 +20598,9 @@
       <c r="K26" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L26" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
@@ -20519,6 +20636,9 @@
       <c r="K27" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L27" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
@@ -20554,6 +20674,9 @@
       <c r="K28" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L28" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
@@ -20589,6 +20712,9 @@
       <c r="K29" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L29" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
@@ -20624,6 +20750,9 @@
       <c r="K30" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L30" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
@@ -20659,6 +20788,9 @@
       <c r="K31" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L31" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
@@ -20694,8 +20826,11 @@
       <c r="K32" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L32" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>128</v>
       </c>
@@ -20729,8 +20864,11 @@
       <c r="K33" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L33" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>704</v>
       </c>
@@ -20765,7 +20903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>749</v>
       </c>
@@ -20800,7 +20938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>1116</v>
       </c>
@@ -20835,7 +20973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>734</v>
       </c>
@@ -20870,7 +21008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>1016</v>
       </c>
@@ -20905,7 +21043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>780</v>
       </c>
@@ -20940,7 +21078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>997</v>
       </c>
@@ -20975,7 +21113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>759</v>
       </c>
@@ -21010,7 +21148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>177</v>
       </c>
@@ -21045,7 +21183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>822</v>
       </c>
@@ -21080,7 +21218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>936</v>
       </c>
@@ -21115,7 +21253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>1117</v>
       </c>
@@ -21150,7 +21288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>609</v>
       </c>
@@ -21185,7 +21323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>982</v>
       </c>
@@ -21220,7 +21358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>677</v>
       </c>
@@ -27032,13 +27170,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(L2))=0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27056,8 +27194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8058A6C-0237-3C45-A728-8864CFB2EE0B}">
   <dimension ref="A1:L343"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27444,6 +27582,9 @@
       <c r="K10" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L10" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -27479,6 +27620,9 @@
       <c r="K11" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L11" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
@@ -27514,6 +27658,9 @@
       <c r="K12" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L12" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
@@ -27549,6 +27696,9 @@
       <c r="K13" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L13" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
@@ -27584,6 +27734,9 @@
       <c r="K14" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L14" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
@@ -27619,6 +27772,9 @@
       <c r="K15" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L15" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
@@ -27654,8 +27810,11 @@
       <c r="K16" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L16" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>697</v>
       </c>
@@ -27689,8 +27848,11 @@
       <c r="K17" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="L17" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>675</v>
       </c>
@@ -27724,8 +27886,11 @@
       <c r="K18" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="L18" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>899</v>
       </c>
@@ -27759,8 +27924,11 @@
       <c r="K19" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L19" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>1292</v>
       </c>
@@ -27794,8 +27962,11 @@
       <c r="K20" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L20" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>1139</v>
       </c>
@@ -27830,7 +28001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>237</v>
       </c>
@@ -27865,7 +28036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>46</v>
       </c>
@@ -27900,7 +28071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>1202</v>
       </c>
@@ -27935,7 +28106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>959</v>
       </c>
@@ -27970,7 +28141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>745</v>
       </c>
@@ -28005,7 +28176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>366</v>
       </c>
@@ -28040,7 +28211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>162</v>
       </c>
@@ -28075,7 +28246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>409</v>
       </c>
@@ -28110,7 +28281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>930</v>
       </c>
@@ -28145,7 +28316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>4</v>
       </c>
@@ -28180,7 +28351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>543</v>
       </c>
@@ -39125,8 +39296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B9B740-1AB9-B944-9990-BD6378BC3535}">
   <dimension ref="A1:L407"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39361,6 +39532,9 @@
       <c r="K6" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L6" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -39396,6 +39570,9 @@
       <c r="K7" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L7" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -39431,6 +39608,9 @@
       <c r="K8" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L8" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -39466,6 +39646,9 @@
       <c r="K9" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L9" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
@@ -39501,6 +39684,9 @@
       <c r="K10" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L10" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -39536,6 +39722,9 @@
       <c r="K11" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L11" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
@@ -39571,6 +39760,9 @@
       <c r="K12" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L12" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
@@ -39606,6 +39798,9 @@
       <c r="K13" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L13" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
@@ -39641,6 +39836,9 @@
       <c r="K14" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L14" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
@@ -39676,6 +39874,9 @@
       <c r="K15" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L15" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
@@ -39711,8 +39912,11 @@
       <c r="K16" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L16" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>318</v>
       </c>
@@ -39746,8 +39950,11 @@
       <c r="K17" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L17" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>848</v>
       </c>
@@ -39781,8 +39988,11 @@
       <c r="K18" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L18" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>182</v>
       </c>
@@ -39816,8 +40026,11 @@
       <c r="K19" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L19" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>730</v>
       </c>
@@ -39851,8 +40064,11 @@
       <c r="K20" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L20" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>1364</v>
       </c>
@@ -39886,8 +40102,11 @@
       <c r="K21" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+      <c r="L21" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>1074</v>
       </c>
@@ -39921,8 +40140,11 @@
       <c r="K22" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L22" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>27</v>
       </c>
@@ -39957,7 +40179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>1096</v>
       </c>
@@ -39992,7 +40214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>69</v>
       </c>
@@ -40027,7 +40249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>1170</v>
       </c>
@@ -40062,7 +40284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>1137</v>
       </c>
@@ -40097,7 +40319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>1032</v>
       </c>
@@ -40132,7 +40354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>615</v>
       </c>
@@ -40167,7 +40389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>952</v>
       </c>
@@ -40202,7 +40424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>1281</v>
       </c>
@@ -40237,7 +40459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>345</v>
       </c>
@@ -53422,8 +53644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CC2C2B-0A10-3A4E-8484-9B93BC4E9E6B}">
   <dimension ref="A1:L414"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -53620,6 +53842,9 @@
       <c r="K5" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L5" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
@@ -53655,6 +53880,9 @@
       <c r="K6" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L6" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -53690,6 +53918,9 @@
       <c r="K7" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L7" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -53725,6 +53956,9 @@
       <c r="K8" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L8" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -53760,6 +53994,9 @@
       <c r="K9" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L9" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
@@ -53795,6 +54032,9 @@
       <c r="K10" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L10" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -53830,6 +54070,9 @@
       <c r="K11" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L11" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
@@ -53865,6 +54108,9 @@
       <c r="K12" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L12" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
@@ -53899,6 +54145,9 @@
       </c>
       <c r="K13" s="6" t="b">
         <v>1</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>4579</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="51" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Big changes from ESA travel period
Added approx 30 articles, re-wrote manuscript draft
</commit_message>
<xml_diff>
--- a/Randomisation/Final_Randomisation.xlsx
+++ b/Randomisation/Final_Randomisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saoirsekelleher/Documents/Research/QAEco/DOM_Review/Randomisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CF4A3C-BB8D-2C4D-9E71-97AF825625E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F579C0-8CED-BA42-BB7E-B6BB15FB62B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{3B957EFC-CA0F-9A4A-8B5B-5DFB75D21C9C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3B957EFC-CA0F-9A4A-8B5B-5DFB75D21C9C}"/>
   </bookViews>
   <sheets>
     <sheet name="2004-2007" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7542" uniqueCount="4581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7649" uniqueCount="4583">
   <si>
     <t>Review_ID</t>
   </si>
@@ -13798,6 +13798,12 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>&lt;- do next round</t>
+  </si>
+  <si>
+    <t>&lt;- try  and get access</t>
   </si>
 </sst>
 </file>
@@ -14844,8 +14850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085D3674-2ED6-F04D-977B-AC5353E9040B}">
   <dimension ref="A1:L1470"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16945,6 +16951,9 @@
       <c r="K55" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L55" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="56" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
@@ -16980,6 +16989,9 @@
       <c r="K56" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L56" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="57" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
@@ -17015,6 +17027,9 @@
       <c r="K57" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L57" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="58" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
@@ -17050,6 +17065,9 @@
       <c r="K58" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L58" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="59" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
@@ -17085,6 +17103,9 @@
       <c r="K59" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L59" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="60" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
@@ -17120,6 +17141,9 @@
       <c r="K60" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L60" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="61" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
@@ -17155,6 +17179,9 @@
       <c r="K61" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L61" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="62" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
@@ -17190,6 +17217,9 @@
       <c r="K62" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L62" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="63" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
@@ -17225,6 +17255,9 @@
       <c r="K63" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L63" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="64" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
@@ -17260,8 +17293,11 @@
       <c r="K64" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L64" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>312</v>
       </c>
@@ -17295,8 +17331,11 @@
       <c r="K65" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L65" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>25</v>
       </c>
@@ -17330,8 +17369,11 @@
       <c r="K66" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L66" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>688</v>
       </c>
@@ -17365,8 +17407,11 @@
       <c r="K67" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L67" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>762</v>
       </c>
@@ -17400,8 +17445,11 @@
       <c r="K68" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L68" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>616</v>
       </c>
@@ -17435,8 +17483,11 @@
       <c r="K69" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L69" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>760</v>
       </c>
@@ -17470,8 +17521,11 @@
       <c r="K70" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L70" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>12</v>
       </c>
@@ -17505,8 +17559,11 @@
       <c r="K71" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L71" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>311</v>
       </c>
@@ -17540,8 +17597,11 @@
       <c r="K72" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L72" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>1296</v>
       </c>
@@ -17575,8 +17635,11 @@
       <c r="K73" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L73" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>131</v>
       </c>
@@ -17610,8 +17673,11 @@
       <c r="K74" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L74" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>2</v>
       </c>
@@ -17645,8 +17711,11 @@
       <c r="K75" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L75" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>1217</v>
       </c>
@@ -17680,8 +17749,11 @@
       <c r="K76" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L76" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>5</v>
       </c>
@@ -17715,8 +17787,11 @@
       <c r="K77" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L77" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>765</v>
       </c>
@@ -17750,8 +17825,11 @@
       <c r="K78" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L78" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>985</v>
       </c>
@@ -17785,8 +17863,11 @@
       <c r="K79" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L79" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>666</v>
       </c>
@@ -17820,8 +17901,11 @@
       <c r="K80" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L80" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
         <v>580</v>
       </c>
@@ -17855,8 +17939,11 @@
       <c r="K81" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L81" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
         <v>949</v>
       </c>
@@ -17890,8 +17977,11 @@
       <c r="K82" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L82" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
         <v>686</v>
       </c>
@@ -17925,8 +18015,11 @@
       <c r="K83" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L83" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>701</v>
       </c>
@@ -17960,8 +18053,11 @@
       <c r="K84" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L84" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
         <v>1000</v>
       </c>
@@ -17995,8 +18091,11 @@
       <c r="K85" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L85" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>22</v>
       </c>
@@ -18030,8 +18129,11 @@
       <c r="K86" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L86" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>732</v>
       </c>
@@ -18065,8 +18167,11 @@
       <c r="K87" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L87" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>887</v>
       </c>
@@ -18100,8 +18205,11 @@
       <c r="K88" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L88" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
         <v>54</v>
       </c>
@@ -18135,8 +18243,11 @@
       <c r="K89" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L89" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
         <v>1151</v>
       </c>
@@ -18170,8 +18281,11 @@
       <c r="K90" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L90" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>834</v>
       </c>
@@ -18205,8 +18319,11 @@
       <c r="K91" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L91" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>871</v>
       </c>
@@ -18240,8 +18357,11 @@
       <c r="K92" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L92" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
         <v>751</v>
       </c>
@@ -18275,8 +18395,11 @@
       <c r="K93" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L93" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>654</v>
       </c>
@@ -18310,8 +18433,11 @@
       <c r="K94" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L94" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>678</v>
       </c>
@@ -18345,8 +18471,11 @@
       <c r="K95" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L95" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>695</v>
       </c>
@@ -18380,8 +18509,11 @@
       <c r="K96" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L96" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>231</v>
       </c>
@@ -18414,6 +18546,9 @@
       </c>
       <c r="K97" s="6" t="b">
         <v>0</v>
+      </c>
+      <c r="L97" s="6" t="s">
+        <v>4580</v>
       </c>
     </row>
     <row r="310" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -19600,10 +19735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719613DA-2E8B-AC4E-A768-CCAA40374210}">
-  <dimension ref="A1:L213"/>
+  <dimension ref="A1:M213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20902,6 +21037,9 @@
       <c r="K34" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L34" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
@@ -20937,6 +21075,9 @@
       <c r="K35" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L35" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
@@ -20972,6 +21113,9 @@
       <c r="K36" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L36" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
@@ -21007,6 +21151,9 @@
       <c r="K37" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L37" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
@@ -21042,6 +21189,9 @@
       <c r="K38" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L38" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
@@ -21077,6 +21227,9 @@
       <c r="K39" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L39" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
@@ -21112,6 +21265,9 @@
       <c r="K40" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L40" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
@@ -21147,6 +21303,9 @@
       <c r="K41" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L41" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
@@ -21182,6 +21341,9 @@
       <c r="K42" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L42" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
@@ -21217,6 +21379,9 @@
       <c r="K43" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L43" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
@@ -21252,6 +21417,9 @@
       <c r="K44" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L44" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
@@ -21287,6 +21455,9 @@
       <c r="K45" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L45" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
@@ -21322,6 +21493,9 @@
       <c r="K46" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L46" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
@@ -21357,6 +21531,9 @@
       <c r="K47" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L47" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
@@ -21392,8 +21569,11 @@
       <c r="K48" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L48" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>983</v>
       </c>
@@ -21427,8 +21607,11 @@
       <c r="K49" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L49" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>832</v>
       </c>
@@ -21462,8 +21645,11 @@
       <c r="K50" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L50" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>157</v>
       </c>
@@ -21497,8 +21683,11 @@
       <c r="K51" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L51" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>1090</v>
       </c>
@@ -21532,8 +21721,11 @@
       <c r="K52" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L52" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>685</v>
       </c>
@@ -21567,8 +21759,11 @@
       <c r="K53" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L53" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>824</v>
       </c>
@@ -21602,8 +21797,11 @@
       <c r="K54" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L54" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>831</v>
       </c>
@@ -21637,8 +21835,11 @@
       <c r="K55" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L55" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>1381</v>
       </c>
@@ -21672,8 +21873,11 @@
       <c r="K56" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L56" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>297</v>
       </c>
@@ -21707,8 +21911,11 @@
       <c r="K57" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="L57" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>1429</v>
       </c>
@@ -21742,8 +21949,11 @@
       <c r="K58" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L58" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>1148</v>
       </c>
@@ -21777,8 +21987,11 @@
       <c r="K59" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L59" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>1038</v>
       </c>
@@ -21812,8 +22025,11 @@
       <c r="K60" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L60" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>600</v>
       </c>
@@ -21847,8 +22063,11 @@
       <c r="K61" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L61" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>34</v>
       </c>
@@ -21882,8 +22101,14 @@
       <c r="K62" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L62" s="6" t="s">
+        <v>4579</v>
+      </c>
+      <c r="M62" t="s">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>53</v>
       </c>
@@ -21918,7 +22143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>1182</v>
       </c>
@@ -27194,8 +27419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8058A6C-0237-3C45-A728-8864CFB2EE0B}">
   <dimension ref="A1:L343"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28000,6 +28225,9 @@
       <c r="K21" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L21" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
@@ -28035,6 +28263,9 @@
       <c r="K22" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L22" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
@@ -28070,6 +28301,9 @@
       <c r="K23" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L23" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
@@ -28105,6 +28339,9 @@
       <c r="K24" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L24" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
@@ -28140,6 +28377,9 @@
       <c r="K25" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L25" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
@@ -28175,6 +28415,9 @@
       <c r="K26" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L26" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
@@ -28210,6 +28453,9 @@
       <c r="K27" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L27" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
@@ -28244,6 +28490,9 @@
       </c>
       <c r="K28" s="6" t="b">
         <v>1</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>4579</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -39296,8 +39545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B9B740-1AB9-B944-9990-BD6378BC3535}">
   <dimension ref="A1:L407"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40178,6 +40427,9 @@
       <c r="K23" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L23" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
@@ -40213,6 +40465,9 @@
       <c r="K24" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L24" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
@@ -40248,6 +40503,9 @@
       <c r="K25" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L25" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
@@ -40283,6 +40541,9 @@
       <c r="K26" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L26" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
@@ -40318,6 +40579,9 @@
       <c r="K27" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L27" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
@@ -40353,6 +40617,9 @@
       <c r="K28" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L28" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
@@ -40388,6 +40655,9 @@
       <c r="K29" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L29" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
@@ -40423,6 +40693,9 @@
       <c r="K30" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L30" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
@@ -40458,6 +40731,9 @@
       <c r="K31" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L31" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
@@ -40493,8 +40769,11 @@
       <c r="K32" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L32" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>165</v>
       </c>
@@ -40528,8 +40807,11 @@
       <c r="K33" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L33" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>43</v>
       </c>
@@ -40563,8 +40845,11 @@
       <c r="K34" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L34" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>144</v>
       </c>
@@ -40598,8 +40883,11 @@
       <c r="K35" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L35" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>956</v>
       </c>
@@ -40633,8 +40921,11 @@
       <c r="K36" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L36" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>913</v>
       </c>
@@ -40668,8 +40959,11 @@
       <c r="K37" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L37" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>18</v>
       </c>
@@ -40703,8 +40997,11 @@
       <c r="K38" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L38" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>925</v>
       </c>
@@ -40739,7 +41036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>291</v>
       </c>
@@ -40774,7 +41071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>208</v>
       </c>
@@ -40809,7 +41106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>360</v>
       </c>
@@ -40844,7 +41141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>1245</v>
       </c>
@@ -40879,7 +41176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>1458</v>
       </c>
@@ -40914,7 +41211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>787</v>
       </c>
@@ -40949,7 +41246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>866</v>
       </c>
@@ -40984,7 +41281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>1368</v>
       </c>
@@ -41019,7 +41316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>634</v>
       </c>
@@ -53642,10 +53939,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CC2C2B-0A10-3A4E-8484-9B93BC4E9E6B}">
-  <dimension ref="A1:L414"/>
+  <dimension ref="A1:M414"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -54184,6 +54481,9 @@
       <c r="K14" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L14" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
@@ -54219,6 +54519,9 @@
       <c r="K15" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L15" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
@@ -54254,8 +54557,11 @@
       <c r="K16" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L16" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>1305</v>
       </c>
@@ -54289,8 +54595,11 @@
       <c r="K17" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L17" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>1299</v>
       </c>
@@ -54324,8 +54633,11 @@
       <c r="K18" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L18" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>154</v>
       </c>
@@ -54359,8 +54671,11 @@
       <c r="K19" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L19" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>555</v>
       </c>
@@ -54394,8 +54709,11 @@
       <c r="K20" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L20" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>488</v>
       </c>
@@ -54429,8 +54747,11 @@
       <c r="K21" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>1442</v>
       </c>
@@ -54464,8 +54785,11 @@
       <c r="K22" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L22" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>521</v>
       </c>
@@ -54499,8 +54823,11 @@
       <c r="K23" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L23" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>415</v>
       </c>
@@ -54535,7 +54862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>1446</v>
       </c>
@@ -54570,7 +54897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>315</v>
       </c>
@@ -54605,7 +54932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>353</v>
       </c>
@@ -54640,7 +54967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>1336</v>
       </c>
@@ -54675,7 +55002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>1431</v>
       </c>
@@ -54710,7 +55037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>1237</v>
       </c>
@@ -54745,7 +55072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>1388</v>
       </c>
@@ -54780,7 +55107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>1353</v>
       </c>

</xml_diff>

<commit_message>
Added up to 68
</commit_message>
<xml_diff>
--- a/Randomisation/Final_Randomisation.xlsx
+++ b/Randomisation/Final_Randomisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saoirsekelleher/Documents/Research/QAEco/DOM_Review/Randomisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B2E8CC-6014-D941-A0C9-C98BB89FD2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BCFD92-6F4C-0640-AAF1-E1ACC0916F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{3B957EFC-CA0F-9A4A-8B5B-5DFB75D21C9C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{3B957EFC-CA0F-9A4A-8B5B-5DFB75D21C9C}"/>
   </bookViews>
   <sheets>
     <sheet name="2004-2007" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7649" uniqueCount="4582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7657" uniqueCount="4581">
   <si>
     <t>Review_ID</t>
   </si>
@@ -13798,9 +13798,6 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>&lt;- try  and get access</t>
   </si>
 </sst>
 </file>
@@ -14847,7 +14844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085D3674-2ED6-F04D-977B-AC5353E9040B}">
   <dimension ref="A1:L1470"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
+    <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
@@ -19734,8 +19731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719613DA-2E8B-AC4E-A768-CCAA40374210}">
   <dimension ref="A1:L213"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22135,6 +22132,9 @@
       </c>
       <c r="K63" s="6" t="b">
         <v>1</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>4579</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -27413,8 +27413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8058A6C-0237-3C45-A728-8864CFB2EE0B}">
   <dimension ref="A1:L343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28561,6 +28561,9 @@
       <c r="K30" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L30" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
@@ -28596,6 +28599,9 @@
       <c r="K31" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="L31" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
@@ -28630,6 +28636,9 @@
       </c>
       <c r="K32" s="6" t="b">
         <v>1</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>4579</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="85" x14ac:dyDescent="0.2">
@@ -39542,8 +39551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B9B740-1AB9-B944-9990-BD6378BC3535}">
   <dimension ref="A1:L407"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41032,6 +41041,9 @@
       <c r="K39" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L39" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
@@ -41067,6 +41079,9 @@
       <c r="K40" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L40" s="6" t="s">
+        <v>4579</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
@@ -41101,6 +41116,9 @@
       </c>
       <c r="K41" s="6" t="b">
         <v>0</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>4579</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -53931,15 +53949,16 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CC2C2B-0A10-3A4E-8484-9B93BC4E9E6B}">
-  <dimension ref="A1:M414"/>
+  <dimension ref="A1:L414"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -54558,7 +54577,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>1305</v>
       </c>
@@ -54596,7 +54615,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>1299</v>
       </c>
@@ -54634,7 +54653,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>154</v>
       </c>
@@ -54672,7 +54691,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>555</v>
       </c>
@@ -54710,7 +54729,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>488</v>
       </c>
@@ -54744,11 +54763,11 @@
       <c r="K21" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="M21" t="s">
-        <v>4581</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="L21" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>1442</v>
       </c>
@@ -54786,7 +54805,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>521</v>
       </c>
@@ -54824,7 +54843,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>415</v>
       </c>
@@ -54858,8 +54877,11 @@
       <c r="K24" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="L24" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>1446</v>
       </c>
@@ -54894,7 +54916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>315</v>
       </c>
@@ -54929,7 +54951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>353</v>
       </c>
@@ -54964,7 +54986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>1336</v>
       </c>
@@ -54999,7 +55021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>1431</v>
       </c>
@@ -55034,7 +55056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>1237</v>
       </c>
@@ -55069,7 +55091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>1388</v>
       </c>
@@ -55104,7 +55126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>1353</v>
       </c>

</xml_diff>

<commit_message>
Completed up to 72
</commit_message>
<xml_diff>
--- a/Randomisation/Final_Randomisation.xlsx
+++ b/Randomisation/Final_Randomisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saoirsekelleher/Documents/Research/QAEco/DOM_Review/Randomisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BCFD92-6F4C-0640-AAF1-E1ACC0916F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99F36B0-942D-4846-88A2-8A2A49D2CB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{3B957EFC-CA0F-9A4A-8B5B-5DFB75D21C9C}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7657" uniqueCount="4581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7669" uniqueCount="4581">
   <si>
     <t>Review_ID</t>
   </si>
@@ -19731,8 +19731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719613DA-2E8B-AC4E-A768-CCAA40374210}">
   <dimension ref="A1:L213"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22171,8 +22171,11 @@
       <c r="K64" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L64" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>658</v>
       </c>
@@ -22206,8 +22209,11 @@
       <c r="K65" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="L65" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>1428</v>
       </c>
@@ -22241,8 +22247,11 @@
       <c r="K66" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L66" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>665</v>
       </c>
@@ -22276,8 +22285,11 @@
       <c r="K67" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L67" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>1118</v>
       </c>
@@ -22311,8 +22323,11 @@
       <c r="K68" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="L68" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>980</v>
       </c>
@@ -22346,8 +22361,11 @@
       <c r="K69" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L69" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>373</v>
       </c>
@@ -22381,8 +22399,11 @@
       <c r="K70" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L70" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>585</v>
       </c>
@@ -22417,7 +22438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>164</v>
       </c>
@@ -22452,7 +22473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>1214</v>
       </c>
@@ -22487,7 +22508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>309</v>
       </c>
@@ -22522,7 +22543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>823</v>
       </c>
@@ -22557,7 +22578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>719</v>
       </c>
@@ -22592,7 +22613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>298</v>
       </c>
@@ -22627,7 +22648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>127</v>
       </c>
@@ -22662,7 +22683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>963</v>
       </c>
@@ -22697,7 +22718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>811</v>
       </c>
@@ -27413,8 +27434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8058A6C-0237-3C45-A728-8864CFB2EE0B}">
   <dimension ref="A1:L343"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28641,7 +28662,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>830</v>
       </c>
@@ -28675,8 +28696,11 @@
       <c r="K33" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="L33" s="6" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>707</v>
       </c>
@@ -28710,8 +28734,11 @@
       <c r="K34" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="L34" s="6" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>482</v>
       </c>
@@ -28746,7 +28773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>945</v>
       </c>
@@ -28781,7 +28808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>747</v>
       </c>
@@ -28816,7 +28843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>388</v>
       </c>
@@ -28851,7 +28878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>277</v>
       </c>
@@ -28886,7 +28913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>64</v>
       </c>
@@ -28921,7 +28948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>334</v>
       </c>
@@ -28956,7 +28983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>809</v>
       </c>
@@ -28991,7 +29018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>1174</v>
       </c>
@@ -29026,7 +29053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>61</v>
       </c>
@@ -29061,7 +29088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>14</v>
       </c>
@@ -29096,7 +29123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>109</v>
       </c>
@@ -29131,7 +29158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>1111</v>
       </c>
@@ -29166,7 +29193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>295</v>
       </c>
@@ -39551,8 +39578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B9B740-1AB9-B944-9990-BD6378BC3535}">
   <dimension ref="A1:L407"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41154,6 +41181,9 @@
       </c>
       <c r="K42" s="6" t="b">
         <v>0</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>4579</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="85" x14ac:dyDescent="0.2">
@@ -53957,8 +53987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CC2C2B-0A10-3A4E-8484-9B93BC4E9E6B}">
   <dimension ref="A1:L414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -54915,6 +54945,9 @@
       <c r="K25" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="L25" s="6" t="s">
+        <v>4580</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
@@ -54949,6 +54982,9 @@
       </c>
       <c r="K26" s="6" t="b">
         <v>1</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>4579</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="51" x14ac:dyDescent="0.2">

</xml_diff>